<commit_message>
Changement de l'affichage des absences dans le fichier récapitulatif excel.
</commit_message>
<xml_diff>
--- a/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
+++ b/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Nom/Prénom</t>
   </si>
@@ -33,15 +33,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Absence matin</t>
-  </si>
-  <si>
-    <t>Absence après-midi</t>
-  </si>
-  <si>
-    <t>Commentaires</t>
-  </si>
-  <si>
     <t>Titre repas</t>
   </si>
   <si>
@@ -52,6 +43,12 @@
   </si>
   <si>
     <t>Titre transport</t>
+  </si>
+  <si>
+    <t>Nature absence</t>
+  </si>
+  <si>
+    <t>Nombre jour</t>
   </si>
 </sst>
 </file>
@@ -95,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -103,6 +100,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,22 +418,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="68.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,23 +440,17 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="2">
-        <v>34968</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -486,16 +479,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fusion des onglets du résumé Excel en un seul + Modification de la couverture des compilations pour les assistants RH + Modification des menu d'accès au différentes étapes de compilation.
</commit_message>
<xml_diff>
--- a/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
+++ b/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
@@ -12,8 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330"/>
   </bookViews>
   <sheets>
-    <sheet name="Absence" sheetId="1" r:id="rId1"/>
-    <sheet name="Totaux" sheetId="2" r:id="rId2"/>
+    <sheet name="Totaux et Absences" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -80,12 +79,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -94,14 +108,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -418,80 +432,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction récupération hiérarchie + Ajout des commentaires dans l'export excel des compilations.
</commit_message>
<xml_diff>
--- a/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
+++ b/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\5_Partage\T.Besson\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Nom/Prénom</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Nombre jour</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,9 +452,10 @@
     <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -479,8 +483,11 @@
       <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
       <c r="C2" s="1"/>

</xml_diff>

<commit_message>
Ajout de la régularisation sur les compilations Excel.
</commit_message>
<xml_diff>
--- a/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
+++ b/Symfony/web/Pointage/Modele/PointageRecapModele.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Nom/Prénom</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Forfait déplacement</t>
+  </si>
+  <si>
+    <t>Régularisation</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y1" sqref="A1:Y1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +462,12 @@
     <col min="12" max="12" width="13.140625" style="2"/>
     <col min="13" max="13" width="15" style="2" customWidth="1"/>
     <col min="14" max="25" width="10.5703125" style="2"/>
-    <col min="26" max="1025" width="10.5703125"/>
+    <col min="26" max="27" width="10.5703125"/>
+    <col min="28" max="30" width="10.5703125" style="2"/>
+    <col min="31" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -519,6 +524,15 @@
       </c>
       <c r="Y1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>